<commit_message>
changed formatting for pop
</commit_message>
<xml_diff>
--- a/model/data/NLdemographics.xlsx
+++ b/model/data/NLdemographics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CharlieBoi/Documents/Uni shit/AI/Master/Year 1/Design of MultiAgent Systems/Project/A05-MAS-virus-spreading/model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDC9AEA-13D8-364A-AC1D-0CD88F3E05B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179CF433-223F-4E47-8071-148F7C482818}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4440" yWindow="-20860" windowWidth="17240" windowHeight="13900" activeTab="1" xr2:uid="{14DCA9EF-147E-2C4B-819D-46448032E3FB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="16x16" sheetId="1" r:id="rId1"/>
     <sheet name="4x4" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">75+ </t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Females</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Devided</t>
   </si>
 </sst>
 </file>
@@ -679,15 +685,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE58DEE-1F89-AF40-986D-75337E25FDD1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -697,8 +703,14 @@
       <c r="C1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -708,8 +720,16 @@
       <c r="C2">
         <v>1842315</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>SUM(B2:C2)</f>
+        <v>3775257</v>
+      </c>
+      <c r="E2">
+        <f>ROUND(D2/10000,0)</f>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -719,8 +739,16 @@
       <c r="C3">
         <v>1644723</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">SUM(B3:C3)</f>
+        <v>3335653</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="1">ROUND(D3/10000,0)</f>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -730,8 +758,16 @@
       <c r="C4">
         <v>2890525</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>5786322</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -740,6 +776,14 @@
       </c>
       <c r="C5">
         <v>2381197</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4509315</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>